<commit_message>
Actualizadas tablas para burndown/burnup
</commit_message>
<xml_diff>
--- a/Conocimiento/Sprints y Requisitos/Sprint 2/Gráficas/burndown.xlsx
+++ b/Conocimiento/Sprints y Requisitos/Sprint 2/Gráficas/burndown.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\4 - CUARTO\ISPP\Práctica\Repositorio\ISPP_A4MJ\Conocimiento\Sprints y Requisitos\Sprint 1\Gráfica burndown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\4 - CUARTO\ISPP\Práctica\Repositorio\ISPP_A4MJ\Conocimiento\Sprints y Requisitos\Sprint 2\Gráficas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4776AA6B-2CB6-4356-9EF8-4EC5E3A00441}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A807F5-9BD0-4487-9742-2FC3F682218B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{F0C5C22E-06B9-496E-8153-43CCFFD52FA4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Fecha fin</t>
   </si>
@@ -85,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,13 +116,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -134,10 +146,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,8 +170,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -266,22 +284,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>415</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>345.83333333333331</c:v>
+                  <c:v>354.16666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>276.66666666666663</c:v>
+                  <c:v>283.33333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>207.49999999999994</c:v>
+                  <c:v>212.50000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>138.33333333333326</c:v>
+                  <c:v>141.66666666666674</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69.166666666666586</c:v>
+                  <c:v>70.833333333333414</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -366,19 +384,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>415</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>415</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>277</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>237</c:v>
+                  <c:v>247</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>146</c:v>
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -829,10 +850,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>149</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.5</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -905,13 +926,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>149</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>109</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1300,15 +1318,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Ideal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>SP's Ideal</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="85725" cap="rnd">
@@ -1368,22 +1378,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>415</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>345.83333333333331</c:v>
+                  <c:v>354.16666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>276.66666666666663</c:v>
+                  <c:v>283.33333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>207.49999999999994</c:v>
+                  <c:v>212.50000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>138.33333333333326</c:v>
+                  <c:v>141.66666666666674</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69.166666666666586</c:v>
+                  <c:v>70.833333333333414</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -1402,15 +1412,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>SP's Real</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="85725" cap="rnd">
@@ -1468,19 +1470,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>415</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>415</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>277</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>237</c:v>
+                  <c:v>247</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>146</c:v>
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1512,15 +1517,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Budget</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Budget's Real</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="69850" cap="rnd">
@@ -1580,19 +1577,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>29000</c:v>
+                  <c:v>4640</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24360</c:v>
+                  <c:v>7830</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21170</c:v>
+                  <c:v>10150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18850</c:v>
+                  <c:v>11850</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17110</c:v>
+                  <c:v>13550</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1601,6 +1601,68 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-CE30-4B11-B29C-C3B6847739EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Budget's Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="69850" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="dk1">
+                  <a:tint val="30000"/>
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$8:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5675</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8275</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9575</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F859-4CEC-9EB8-C9A5FD4327EE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1614,8 +1676,66 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="548559080"/>
-        <c:axId val="123748504"/>
+        <c:axId val="422739520"/>
+        <c:axId val="422742144"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>Ideal</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="63500" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:tint val="98500"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:glow rad="139700">
+                      <a:schemeClr val="dk1">
+                        <a:tint val="98500"/>
+                        <a:satMod val="175000"/>
+                        <a:alpha val="14000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$14:$F$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>10875</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-F859-4CEC-9EB8-C9A5FD4327EE}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="308821208"/>
@@ -1865,7 +1985,7 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123748504"/>
+        <c:axId val="422742144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1887,7 +2007,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="3600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:ln w="6350">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
@@ -1904,12 +2024,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="548559080"/>
+        <c:crossAx val="422739520"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="548559080"/>
+        <c:axId val="422739520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1919,7 +2039,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123748504"/>
+        <c:crossAx val="422742144"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3738,14 +3858,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>220915</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>501063</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>180973</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>612321</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>220116</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>54428</xdr:rowOff>
     </xdr:to>
@@ -3811,13 +3931,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>212910</xdr:colOff>
+      <xdr:colOff>1434351</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>78440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>235323</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>246528</xdr:colOff>
       <xdr:row>96</xdr:row>
       <xdr:rowOff>22412</xdr:rowOff>
     </xdr:to>
@@ -4144,10 +4264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4340BF-5239-4811-90B4-33AEB030F494}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4160,7 +4280,7 @@
     <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -4174,7 +4294,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4188,7 +4308,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -4199,28 +4319,29 @@
         <v>14</v>
       </c>
       <c r="E3" s="1">
-        <v>128</v>
+        <f>17+13+10+11+20+20+26+21</f>
+        <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <f>E1+E2+E3</f>
-        <v>415</v>
+        <v>425</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
-        <v>69.166666666666671</v>
+        <v>70.833333333333329</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4236,135 +4357,178 @@
       <c r="E7" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>0</v>
       </c>
       <c r="B8" s="5">
         <f>B4</f>
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="C8" s="5">
         <f>B8</f>
-        <v>415</v>
-      </c>
-      <c r="D8">
-        <v>29000</v>
+        <v>425</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4640</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
       </c>
+      <c r="F8" s="1">
+        <f>B33</f>
+        <v>3075</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>1</v>
       </c>
       <c r="B9" s="5">
         <f>B4-B5</f>
-        <v>345.83333333333331</v>
+        <v>354.16666666666669</v>
       </c>
       <c r="C9" s="5">
         <f>C8-E8</f>
-        <v>415</v>
-      </c>
-      <c r="D9">
-        <v>24360</v>
+        <v>425</v>
+      </c>
+      <c r="D9" s="1">
+        <f>D8+D38</f>
+        <v>7830</v>
       </c>
       <c r="E9" s="5">
         <v>138</v>
       </c>
+      <c r="F9" s="1">
+        <f>B34</f>
+        <v>4375</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>2</v>
       </c>
       <c r="B10" s="5">
         <f>B9-B5</f>
-        <v>276.66666666666663</v>
+        <v>283.33333333333337</v>
       </c>
       <c r="C10" s="5">
         <f>C9-E9</f>
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="D10" s="1">
-        <v>21170</v>
+        <f>D9+D37</f>
+        <v>10150</v>
       </c>
       <c r="E10" s="5">
         <v>40</v>
       </c>
+      <c r="F10" s="5">
+        <f>B35</f>
+        <v>5675</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>3</v>
       </c>
       <c r="B11" s="5">
         <f>B10-B5</f>
-        <v>207.49999999999994</v>
+        <v>212.50000000000006</v>
       </c>
       <c r="C11" s="5">
         <f>C10-E10</f>
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="D11" s="1">
-        <v>18850</v>
+        <f>D10+D35</f>
+        <v>11850</v>
       </c>
       <c r="E11" s="5">
         <v>91</v>
       </c>
+      <c r="F11" s="5">
+        <f>B36</f>
+        <v>6975</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>4</v>
       </c>
       <c r="B12" s="5">
         <f>B11-B5</f>
-        <v>138.33333333333326</v>
+        <v>141.66666666666674</v>
       </c>
       <c r="C12" s="5">
         <f>C11-E11</f>
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D12" s="1">
-        <v>17110</v>
+        <f>D11+D35</f>
+        <v>13550</v>
+      </c>
+      <c r="E12" s="1">
+        <f>18+8+12+15+20+13+13+15</f>
+        <v>114</v>
+      </c>
+      <c r="F12" s="5">
+        <f>B37</f>
+        <v>8275</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>5</v>
       </c>
       <c r="B13" s="1">
         <f>B12-B5</f>
-        <v>69.166666666666586</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+        <v>70.833333333333414</v>
+      </c>
+      <c r="C13" s="1">
+        <f>C12-E12</f>
+        <v>42</v>
+      </c>
+      <c r="D13" s="1">
+        <v>16000</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="5">
+        <f>B38</f>
+        <v>9575</v>
+      </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>6</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="F14" s="5">
+        <f>B39</f>
+        <v>10875</v>
+      </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E15" s="4">
         <v>43171</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
-      <c r="D16" s="5"/>
       <c r="E16" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>
-      <c r="D17" s="5"/>
       <c r="E17" s="4">
         <v>43192</v>
       </c>
@@ -4377,7 +4541,6 @@
         <v>2</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="5"/>
       <c r="E18" s="4" t="s">
         <v>8</v>
       </c>
@@ -4387,10 +4550,9 @@
         <v>3</v>
       </c>
       <c r="B19" s="1">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="5"/>
       <c r="E19" s="4">
         <v>43213</v>
       </c>
@@ -4400,8 +4562,8 @@
         <v>4</v>
       </c>
       <c r="B20" s="1">
-        <f>149/2</f>
-        <v>74.5</v>
+        <f>156/2</f>
+        <v>78</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="5"/>
@@ -4433,12 +4595,12 @@
         <v>0</v>
       </c>
       <c r="B23" s="5">
-        <f>E2</f>
-        <v>149</v>
+        <f>138+18</f>
+        <v>156</v>
       </c>
       <c r="C23" s="5">
         <f>B23</f>
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="D23" s="5">
         <v>0</v>
@@ -4450,14 +4612,15 @@
       </c>
       <c r="B24" s="5">
         <f>B23-B20</f>
-        <v>74.5</v>
+        <v>78</v>
       </c>
       <c r="C24" s="5">
         <f>C23-D24</f>
-        <v>109</v>
-      </c>
-      <c r="D24" s="5">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="D24" s="1">
+        <f>E12</f>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -4468,21 +4631,15 @@
         <f>B24-B20</f>
         <v>0</v>
       </c>
-      <c r="C25" s="5">
-        <f>C24-D25</f>
-        <v>18</v>
-      </c>
-      <c r="D25" s="5">
-        <f>105-14</f>
-        <v>91</v>
-      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="1">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -4490,7 +4647,8 @@
         <v>15</v>
       </c>
       <c r="B29" s="1">
-        <v>29000</v>
+        <f>(29000/16)*6</f>
+        <v>10875</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -4498,8 +4656,7 @@
         <v>16</v>
       </c>
       <c r="B30" s="1">
-        <f>B29/B28</f>
-        <v>1812.5</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -4520,32 +4677,28 @@
       <c r="A33" s="6">
         <v>0</v>
       </c>
-      <c r="B33" s="5">
-        <f>B29</f>
-        <v>29000</v>
-      </c>
-      <c r="C33" s="5">
-        <f>B29</f>
-        <v>29000</v>
-      </c>
-      <c r="D33" s="5">
-        <v>0</v>
-      </c>
+      <c r="B33" s="1">
+        <f>B34-B30</f>
+        <v>3075</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>1</v>
       </c>
-      <c r="B34" s="5">
-        <f>B33-B30</f>
-        <v>27187.5</v>
-      </c>
-      <c r="C34" s="5">
-        <f>C33-D34</f>
-        <v>24360</v>
-      </c>
-      <c r="D34" s="5">
-        <v>4640</v>
+      <c r="B34" s="1">
+        <f>B35-B30</f>
+        <v>4375</v>
+      </c>
+      <c r="C34" s="1">
+        <f>C35-D35</f>
+        <v>-2715</v>
+      </c>
+      <c r="D34" s="1">
+        <f>D13-D12</f>
+        <v>2450</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4553,15 +4706,15 @@
         <v>2</v>
       </c>
       <c r="B35" s="5">
-        <f>B34-B30</f>
-        <v>25375</v>
+        <f>B36-B30</f>
+        <v>5675</v>
       </c>
       <c r="C35" s="5">
-        <f>C34-D35</f>
-        <v>21170</v>
-      </c>
-      <c r="D35" s="5">
-        <v>3190</v>
+        <f>C36-D36</f>
+        <v>-1015</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1700</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4569,15 +4722,15 @@
         <v>3</v>
       </c>
       <c r="B36" s="5">
-        <f>B35-B30</f>
-        <v>23562.5</v>
+        <f>B37-B30</f>
+        <v>6975</v>
       </c>
       <c r="C36" s="5">
-        <f>C35-D36</f>
-        <v>18850</v>
+        <f>C37-D37</f>
+        <v>725</v>
       </c>
       <c r="D36" s="5">
-        <v>2320</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -4585,68 +4738,62 @@
         <v>4</v>
       </c>
       <c r="B37" s="5">
-        <f>B36-B30</f>
-        <v>21750</v>
+        <f>B38-B30</f>
+        <v>8275</v>
       </c>
       <c r="C37" s="5">
-        <f>C36-D37</f>
-        <v>17110</v>
+        <f>C38-D38</f>
+        <v>3045</v>
       </c>
       <c r="D37" s="5">
-        <v>1740</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>5</v>
       </c>
-      <c r="B38" s="1">
-        <f>B37-B30</f>
-        <v>19937.5</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="B38" s="5">
+        <f>B39-B30</f>
+        <v>9575</v>
+      </c>
+      <c r="C38" s="5">
+        <f>C39-D39</f>
+        <v>6235</v>
+      </c>
+      <c r="D38" s="5">
+        <v>3190</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>6</v>
       </c>
-      <c r="B39" s="1">
-        <f>B38-B30</f>
-        <v>18125</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
+      <c r="B39" s="5">
+        <f>B29</f>
+        <v>10875</v>
+      </c>
+      <c r="C39" s="5">
+        <f>B29</f>
+        <v>10875</v>
+      </c>
+      <c r="D39" s="5">
+        <v>4640</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="6"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="6"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="6"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="D41" s="5"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="6"/>
       <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="3"/>

</xml_diff>